<commit_message>
Cập nhật database. Cập nhật frmHocSinh, frmGiaoVien. frmLogin chưa có cái qq gì hết
</commit_message>
<xml_diff>
--- a/Đề toán.xlsx
+++ b/Đề toán.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lập trình\Năm 4 - HK1\Lập trình ứng dụng quản lý 1\DA-LTUDQL1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\DA-LTUDQL1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8062802-2CE7-4E6B-A498-64E970AC3C93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA271B28-5319-4C75-8E90-DEDAE5414100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CauHoi" sheetId="2" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>Cho elip (E): (x^2/25)+(y^2/9)=1. Đường thẳng (d): x=-4 cắt (E) tại hai điểm M,N. Khi đó:</t>
   </si>
   <si>
-    <t>CHO elip (E): (x^2/16)+(y^2/9)=1. M là điểm nằm trên (E). Lúc đó đoạn thẳng OM thỏa:</t>
-  </si>
-  <si>
     <t>maDA</t>
   </si>
   <si>
@@ -336,6 +333,9 @@
   </si>
   <si>
     <t>4 &lt;= OM &lt;= 5</t>
+  </si>
+  <si>
+    <t>Cho elip (E): (x^2/16)+(y^2/9)=1. M là điểm nằm trên (E). Lúc đó đoạn thẳng OM thỏa:</t>
   </si>
 </sst>
 </file>
@@ -701,18 +701,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="244.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="244.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -723,7 +723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -734,7 +734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -745,7 +745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -756,7 +756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -767,7 +767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -778,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -789,7 +789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -800,7 +800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -811,7 +811,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -822,7 +822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -833,7 +833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -844,7 +844,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -855,7 +855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -866,7 +866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -877,7 +877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -888,7 +888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -899,7 +899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -910,7 +910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -921,7 +921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -932,12 +932,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -955,30 +955,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0"/>
+    <sheetView topLeftCell="A12" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="67.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="1" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -986,13 +986,13 @@
         <v>425</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1000,13 +1000,13 @@
         <v>426</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1014,13 +1014,13 @@
         <v>427</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1028,13 +1028,13 @@
         <v>428</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1042,13 +1042,13 @@
         <v>429</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1056,13 +1056,13 @@
         <v>430</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1070,13 +1070,13 @@
         <v>431</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1084,13 +1084,13 @@
         <v>432</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1098,13 +1098,13 @@
         <v>433</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1112,13 +1112,13 @@
         <v>434</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1126,13 +1126,13 @@
         <v>435</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1140,13 +1140,13 @@
         <v>436</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1154,13 +1154,13 @@
         <v>437</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1168,13 +1168,13 @@
         <v>438</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>4</v>
       </c>
@@ -1182,13 +1182,13 @@
         <v>439</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1196,13 +1196,13 @@
         <v>440</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>5</v>
       </c>
@@ -1210,13 +1210,13 @@
         <v>441</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>5</v>
       </c>
@@ -1224,13 +1224,13 @@
         <v>442</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>5</v>
       </c>
@@ -1238,13 +1238,13 @@
         <v>443</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>5</v>
       </c>
@@ -1252,13 +1252,13 @@
         <v>444</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>6</v>
       </c>
@@ -1266,13 +1266,13 @@
         <v>445</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>6</v>
       </c>
@@ -1280,13 +1280,13 @@
         <v>446</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>6</v>
       </c>
@@ -1294,13 +1294,13 @@
         <v>447</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>6</v>
       </c>
@@ -1308,13 +1308,13 @@
         <v>448</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>7</v>
       </c>
@@ -1322,13 +1322,13 @@
         <v>449</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1336,13 +1336,13 @@
         <v>450</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>7</v>
       </c>
@@ -1350,13 +1350,13 @@
         <v>451</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D28" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>7</v>
       </c>
@@ -1364,13 +1364,13 @@
         <v>452</v>
       </c>
       <c r="C29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>8</v>
       </c>
@@ -1378,13 +1378,13 @@
         <v>453</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>8</v>
       </c>
@@ -1392,13 +1392,13 @@
         <v>454</v>
       </c>
       <c r="C31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>8</v>
       </c>
@@ -1406,13 +1406,13 @@
         <v>455</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>8</v>
       </c>
@@ -1420,13 +1420,13 @@
         <v>456</v>
       </c>
       <c r="C33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D33" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>9</v>
       </c>
@@ -1434,13 +1434,13 @@
         <v>457</v>
       </c>
       <c r="C34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>9</v>
       </c>
@@ -1448,13 +1448,13 @@
         <v>458</v>
       </c>
       <c r="C35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>9</v>
       </c>
@@ -1462,13 +1462,13 @@
         <v>459</v>
       </c>
       <c r="C36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>9</v>
       </c>
@@ -1476,13 +1476,13 @@
         <v>460</v>
       </c>
       <c r="C37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>10</v>
       </c>
@@ -1490,13 +1490,13 @@
         <v>461</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>10</v>
       </c>
@@ -1504,13 +1504,13 @@
         <v>462</v>
       </c>
       <c r="C39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>10</v>
       </c>
@@ -1518,13 +1518,13 @@
         <v>463</v>
       </c>
       <c r="C40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>10</v>
       </c>
@@ -1532,13 +1532,13 @@
         <v>464</v>
       </c>
       <c r="C41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D41" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>11</v>
       </c>
@@ -1546,13 +1546,13 @@
         <v>465</v>
       </c>
       <c r="C42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>11</v>
       </c>
@@ -1560,13 +1560,13 @@
         <v>466</v>
       </c>
       <c r="C43" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>11</v>
       </c>
@@ -1574,13 +1574,13 @@
         <v>467</v>
       </c>
       <c r="C44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D44" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>11</v>
       </c>
@@ -1588,13 +1588,13 @@
         <v>468</v>
       </c>
       <c r="C45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D45" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>12</v>
       </c>
@@ -1602,13 +1602,13 @@
         <v>469</v>
       </c>
       <c r="C46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D46" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>12</v>
       </c>
@@ -1616,13 +1616,13 @@
         <v>470</v>
       </c>
       <c r="C47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>12</v>
       </c>
@@ -1630,13 +1630,13 @@
         <v>471</v>
       </c>
       <c r="C48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D48" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>12</v>
       </c>
@@ -1644,13 +1644,13 @@
         <v>472</v>
       </c>
       <c r="C49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>13</v>
       </c>
@@ -1658,13 +1658,13 @@
         <v>473</v>
       </c>
       <c r="C50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D50" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>13</v>
       </c>
@@ -1672,13 +1672,13 @@
         <v>474</v>
       </c>
       <c r="C51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D51" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>13</v>
       </c>
@@ -1686,13 +1686,13 @@
         <v>475</v>
       </c>
       <c r="C52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D52" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>13</v>
       </c>
@@ -1700,13 +1700,13 @@
         <v>476</v>
       </c>
       <c r="C53" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D53" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>14</v>
       </c>
@@ -1714,13 +1714,13 @@
         <v>477</v>
       </c>
       <c r="C54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D54" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>14</v>
       </c>
@@ -1728,13 +1728,13 @@
         <v>478</v>
       </c>
       <c r="C55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D55" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>14</v>
       </c>
@@ -1742,13 +1742,13 @@
         <v>479</v>
       </c>
       <c r="C56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D56" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>14</v>
       </c>
@@ -1756,13 +1756,13 @@
         <v>480</v>
       </c>
       <c r="C57" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>15</v>
       </c>
@@ -1770,13 +1770,13 @@
         <v>481</v>
       </c>
       <c r="C58" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>15</v>
       </c>
@@ -1784,13 +1784,13 @@
         <v>482</v>
       </c>
       <c r="C59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D59" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>15</v>
       </c>
@@ -1798,13 +1798,13 @@
         <v>483</v>
       </c>
       <c r="C60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D60" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>15</v>
       </c>
@@ -1812,13 +1812,13 @@
         <v>484</v>
       </c>
       <c r="C61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D61" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>16</v>
       </c>
@@ -1826,13 +1826,13 @@
         <v>485</v>
       </c>
       <c r="C62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>16</v>
       </c>
@@ -1840,13 +1840,13 @@
         <v>486</v>
       </c>
       <c r="C63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>16</v>
       </c>
@@ -1854,13 +1854,13 @@
         <v>487</v>
       </c>
       <c r="C64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D64" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>16</v>
       </c>
@@ -1868,13 +1868,13 @@
         <v>488</v>
       </c>
       <c r="C65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>17</v>
       </c>
@@ -1882,13 +1882,13 @@
         <v>489</v>
       </c>
       <c r="C66" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>17</v>
       </c>
@@ -1896,13 +1896,13 @@
         <v>490</v>
       </c>
       <c r="C67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D67" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>17</v>
       </c>
@@ -1910,13 +1910,13 @@
         <v>491</v>
       </c>
       <c r="C68" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D68" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>17</v>
       </c>
@@ -1924,13 +1924,13 @@
         <v>492</v>
       </c>
       <c r="C69" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D69" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>18</v>
       </c>
@@ -1938,13 +1938,13 @@
         <v>493</v>
       </c>
       <c r="C70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D70" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>18</v>
       </c>
@@ -1952,13 +1952,13 @@
         <v>494</v>
       </c>
       <c r="C71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D71" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>18</v>
       </c>
@@ -1966,13 +1966,13 @@
         <v>495</v>
       </c>
       <c r="C72" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D72" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>18</v>
       </c>
@@ -1980,13 +1980,13 @@
         <v>496</v>
       </c>
       <c r="C73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>19</v>
       </c>
@@ -1994,13 +1994,13 @@
         <v>497</v>
       </c>
       <c r="C74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D74" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>19</v>
       </c>
@@ -2008,13 +2008,13 @@
         <v>498</v>
       </c>
       <c r="C75" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D75" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>19</v>
       </c>
@@ -2022,13 +2022,13 @@
         <v>499</v>
       </c>
       <c r="C76" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D76" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>19</v>
       </c>
@@ -2036,13 +2036,13 @@
         <v>500</v>
       </c>
       <c r="C77" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D77" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>20</v>
       </c>
@@ -2050,13 +2050,13 @@
         <v>501</v>
       </c>
       <c r="C78" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D78" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>20</v>
       </c>
@@ -2064,13 +2064,13 @@
         <v>502</v>
       </c>
       <c r="C79" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D79" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>20</v>
       </c>
@@ -2078,13 +2078,13 @@
         <v>503</v>
       </c>
       <c r="C80" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D80" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>20</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>504</v>
       </c>
       <c r="C81" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D81" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Hoan thanh them tab QuanLyDeThi, frmLogin
</commit_message>
<xml_diff>
--- a/Đề toán.xlsx
+++ b/Đề toán.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\DA-LTUDQL1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lập trình\Năm 4 - HK1\Lập trình ứng dụng quản lý 1\DA-LTUDQL1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA271B28-5319-4C75-8E90-DEDAE5414100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B2BE0C-76B3-4B65-BF3B-2BAD63CBB8E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CauHoi" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="108">
   <si>
     <t>maCH</t>
   </si>
@@ -336,16 +336,33 @@
   </si>
   <si>
     <t>Cho elip (E): (x^2/16)+(y^2/9)=1. M là điểm nằm trên (E). Lúc đó đoạn thẳng OM thỏa:</t>
+  </si>
+  <si>
+    <t>maMH</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>maKhoi</t>
+  </si>
+  <si>
+    <t>K10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -390,12 +407,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C21" totalsRowShown="0">
-  <autoFilter ref="A1:C21" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E21" totalsRowShown="0">
+  <autoFilter ref="A1:E21" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="maCH"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NoiDung"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="maCD"/>
+    <tableColumn id="4" xr3:uid="{5F9507A9-6127-46FE-8AE6-302751C22408}" name="maMH"/>
+    <tableColumn id="5" xr3:uid="{6BE48C43-27AC-48E5-9B18-63CC015FBFDD}" name="maKhoi"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -699,20 +718,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
-    <col min="2" max="2" width="244.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="244.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -722,8 +742,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -733,8 +759,14 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -744,8 +776,14 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -755,8 +793,14 @@
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -766,8 +810,14 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -777,8 +827,14 @@
       <c r="C6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -788,8 +844,14 @@
       <c r="C7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -799,8 +861,14 @@
       <c r="C8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -810,8 +878,14 @@
       <c r="C9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -821,8 +895,14 @@
       <c r="C10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -832,8 +912,14 @@
       <c r="C11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -843,8 +929,14 @@
       <c r="C12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -854,8 +946,14 @@
       <c r="C13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -865,8 +963,14 @@
       <c r="C14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -876,8 +980,14 @@
       <c r="C15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -887,8 +997,14 @@
       <c r="C16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -898,8 +1014,14 @@
       <c r="C17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -909,8 +1031,14 @@
       <c r="C18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -920,8 +1048,14 @@
       <c r="C19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -931,8 +1065,14 @@
       <c r="C20">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -942,8 +1082,15 @@
       <c r="C21">
         <v>4</v>
       </c>
+      <c r="D21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" t="s">
+        <v>107</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -957,14 +1104,14 @@
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="3" width="67.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+    <col min="1" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="67.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -978,7 +1125,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -992,7 +1139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1006,7 +1153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1020,7 +1167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1034,7 +1181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1048,7 +1195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1062,7 +1209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1076,7 +1223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1090,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1104,7 +1251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1118,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1132,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1146,7 +1293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1160,7 +1307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1174,7 +1321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -1188,7 +1335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1202,7 +1349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -1216,7 +1363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
@@ -1230,7 +1377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -1244,7 +1391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>5</v>
       </c>
@@ -1258,7 +1405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6</v>
       </c>
@@ -1272,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6</v>
       </c>
@@ -1286,7 +1433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6</v>
       </c>
@@ -1300,7 +1447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
@@ -1314,7 +1461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>7</v>
       </c>
@@ -1328,7 +1475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1342,7 +1489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7</v>
       </c>
@@ -1356,7 +1503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7</v>
       </c>
@@ -1370,7 +1517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>8</v>
       </c>
@@ -1384,7 +1531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>8</v>
       </c>
@@ -1398,7 +1545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>8</v>
       </c>
@@ -1412,7 +1559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>8</v>
       </c>
@@ -1426,7 +1573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>9</v>
       </c>
@@ -1440,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>9</v>
       </c>
@@ -1454,7 +1601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>9</v>
       </c>
@@ -1468,7 +1615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>9</v>
       </c>
@@ -1482,7 +1629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>10</v>
       </c>
@@ -1496,7 +1643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>10</v>
       </c>
@@ -1510,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>10</v>
       </c>
@@ -1524,7 +1671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>10</v>
       </c>
@@ -1538,7 +1685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>11</v>
       </c>
@@ -1552,7 +1699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>11</v>
       </c>
@@ -1566,7 +1713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>11</v>
       </c>
@@ -1580,7 +1727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>11</v>
       </c>
@@ -1594,7 +1741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>12</v>
       </c>
@@ -1608,7 +1755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>12</v>
       </c>
@@ -1622,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>12</v>
       </c>
@@ -1636,7 +1783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>12</v>
       </c>
@@ -1650,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>13</v>
       </c>
@@ -1664,7 +1811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>13</v>
       </c>
@@ -1678,7 +1825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>13</v>
       </c>
@@ -1692,7 +1839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>13</v>
       </c>
@@ -1706,7 +1853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>14</v>
       </c>
@@ -1720,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>14</v>
       </c>
@@ -1734,7 +1881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>14</v>
       </c>
@@ -1748,7 +1895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>14</v>
       </c>
@@ -1762,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>15</v>
       </c>
@@ -1776,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>15</v>
       </c>
@@ -1790,7 +1937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>15</v>
       </c>
@@ -1804,7 +1951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>15</v>
       </c>
@@ -1818,7 +1965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>16</v>
       </c>
@@ -1832,7 +1979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>16</v>
       </c>
@@ -1846,7 +1993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>16</v>
       </c>
@@ -1860,7 +2007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>16</v>
       </c>
@@ -1874,7 +2021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>17</v>
       </c>
@@ -1888,7 +2035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>17</v>
       </c>
@@ -1902,7 +2049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>17</v>
       </c>
@@ -1916,7 +2063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>17</v>
       </c>
@@ -1930,7 +2077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>18</v>
       </c>
@@ -1944,7 +2091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>18</v>
       </c>
@@ -1958,7 +2105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>18</v>
       </c>
@@ -1972,7 +2119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>18</v>
       </c>
@@ -1986,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>19</v>
       </c>
@@ -2000,7 +2147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>19</v>
       </c>
@@ -2014,7 +2161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>19</v>
       </c>
@@ -2028,7 +2175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>19</v>
       </c>
@@ -2042,7 +2189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>20</v>
       </c>
@@ -2056,7 +2203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>20</v>
       </c>
@@ -2070,7 +2217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>20</v>
       </c>
@@ -2084,7 +2231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>20</v>
       </c>

</xml_diff>